<commit_message>
Adding some missing Customer requirments
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Doc/CRS .xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Doc/CRS .xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Costumer Requirement ID</t>
   </si>
@@ -74,28 +74,67 @@
     <t xml:space="preserve">The system should be Initialized at the current temperature and the fan speed </t>
   </si>
   <si>
-    <t xml:space="preserve">The system should has available menue to control Temperature or Fan speed . If user select temperature option he can increase or decrease the temperature. If user select fan speed option he can increase or decrease the fan speed .
+    <t>CRS_001</t>
+  </si>
+  <si>
+    <t>CRS_002</t>
+  </si>
+  <si>
+    <t>CRS_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system should has available menu to control Temperature or Fan speed . If user select temperature option he can increase or decrease the temperature. If user select fan speed option he can increase or decrease the fan speed .
 </t>
   </si>
   <si>
-    <t>CRS_001</t>
-  </si>
-  <si>
-    <t>CRS_002</t>
-  </si>
-  <si>
-    <t>CRS_003</t>
+    <t>CRS_004</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>LCD size is 16x2</t>
+  </si>
+  <si>
+    <t>CRS_005</t>
+  </si>
+  <si>
+    <t>Fan speed and temperature range should be configurble by user</t>
+  </si>
+  <si>
+    <t>CRS_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there are 4 buttons                                                                                                                                                            1- Selection Button
+2-Increase Button
+3-Decrease Button
+4-On/Off Button        </t>
+  </si>
+  <si>
+    <t>CRS_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the whole system should be portable </t>
+  </si>
+  <si>
+    <t>CRS_008</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the used switch is tactile switch </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -103,7 +142,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -111,14 +150,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -126,7 +165,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -134,7 +173,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -177,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -235,26 +282,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -275,20 +302,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -300,12 +333,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -320,15 +350,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -344,37 +368,48 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -437,7 +472,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -472,7 +507,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -681,177 +716,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="37.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="37.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="40" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="25"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="25"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="C8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="C9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>25</v>
+      </c>
       <c r="D10"/>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11"/>
+    <row r="11" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>27</v>
+      </c>
       <c r="D11"/>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="25"/>
-      <c r="C12"/>
+    <row r="12" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>29</v>
+      </c>
       <c r="D12"/>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="4"/>
+    <row r="13" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
+  <mergeCells count="2">
     <mergeCell ref="D2:D6"/>
     <mergeCell ref="E2:E6"/>
   </mergeCells>
@@ -868,118 +910,118 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="31"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="31"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="31"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="31"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="31"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="31"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="25"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="26"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Linking between CRS abd SIQ
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Doc/CRS .xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Doc/CRS .xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Costumer Requirement ID</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>The system should has a Button to turn on or off the LCD of the digital air conditioner screen .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The system should be Initialized at the current temperature and the fan speed </t>
   </si>
   <si>
     <t>CRS_001</t>
@@ -124,6 +121,30 @@
   </si>
   <si>
     <t xml:space="preserve">the used switch is tactile switch </t>
+  </si>
+  <si>
+    <t>SIQ ID</t>
+  </si>
+  <si>
+    <t>SIQ_1</t>
+  </si>
+  <si>
+    <t>SIQ_4</t>
+  </si>
+  <si>
+    <t>SIQ_3</t>
+  </si>
+  <si>
+    <t>The system should be Initialized with the last temperature and the fan speed reading before the system powered off</t>
+  </si>
+  <si>
+    <t>SIQ_5</t>
+  </si>
+  <si>
+    <t>SIQ_6</t>
+  </si>
+  <si>
+    <t>SIQ_2</t>
   </si>
 </sst>
 </file>
@@ -377,8 +398,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -398,18 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -718,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -747,8 +768,8 @@
       <c r="C2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
@@ -758,22 +779,22 @@
       <c r="C3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="11"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
@@ -785,12 +806,14 @@
       <c r="C6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>14</v>
@@ -803,89 +826,103 @@
     </row>
     <row r="8" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="14"/>
+        <v>38</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>39</v>
+      </c>
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="C10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10"/>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="E10"/>
     </row>
     <row r="11" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11"/>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="E11"/>
     </row>
     <row r="12" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12"/>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E12"/>
     </row>
     <row r="13" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>31</v>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>34</v>
+      <c r="D14" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -893,8 +930,7 @@
       <c r="B15" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D2:D6"/>
+  <mergeCells count="1">
     <mergeCell ref="E2:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -929,92 +965,92 @@
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="5"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="5"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="5"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="34" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="5"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="30"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="5"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="30"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="5"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
-      <c r="B10" s="30"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="5"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
     </row>

</xml_diff>